<commit_message>
Generacion de Ventana Multigraficos
</commit_message>
<xml_diff>
--- a/Definición usuarios.xlsx
+++ b/Definición usuarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Documents\GitHub\Datos-Epilepsia-2021\Jorge Diego Manrique\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvggt-my.sharepoint.com/personal/men19673_uvg_edu_gt/Documents/University/Tesis/Herramienta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A41E5-A792-492C-95CE-35788D115142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{279A41E5-A792-492C-95CE-35788D115142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D0CEAA9-C6D5-4734-BA22-0F05EE5DF338}"/>
   <bookViews>
-    <workbookView xWindow="7245" yWindow="8205" windowWidth="17640" windowHeight="9450" xr2:uid="{09960BBC-791D-4C4A-86A7-0BCEF8ED93A5}"/>
+    <workbookView xWindow="468" yWindow="1872" windowWidth="12612" windowHeight="8928" xr2:uid="{09960BBC-791D-4C4A-86A7-0BCEF8ED93A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Administrador</t>
   </si>
@@ -103,12 +103,48 @@
   <si>
     <t>La tabla "pacientes" contiene columnas confidenciales.</t>
   </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>eeganalysistoolbox@gmail.com</t>
+  </si>
+  <si>
+    <t>cgsw pylb ptlf wvng</t>
+  </si>
+  <si>
+    <t>asunto</t>
+  </si>
+  <si>
+    <t>EEG Analysis Toolbox - Recuperar Contraseña</t>
+  </si>
+  <si>
+    <t>mensaje_1</t>
+  </si>
+  <si>
+    <t>-&gt;</t>
+  </si>
+  <si>
+    <t>mensaje_2</t>
+  </si>
+  <si>
+    <t>Puedes cambiarla en cualquier momento en la pantalla de configuración despues de iniciar sesión.</t>
+  </si>
+  <si>
+    <t>server</t>
+  </si>
+  <si>
+    <t>smtp.gmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +156,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,16 +186,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -168,7 +216,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -464,21 +512,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E865866-EF4E-4B78-9F9B-509577440023}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -489,7 +537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -500,7 +548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -511,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -525,7 +573,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -539,8 +587,59 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{9EA6CC1E-7E15-4D3B-A841-0FFA0CC35452}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>